<commit_message>
Changed to new format with time. Verification of balance is not working for whatever reason yet
</commit_message>
<xml_diff>
--- a/Examples/primer_dlya_soobsheniya_ob_oshibkah_primer_konvertatsii.xlsx
+++ b/Examples/primer_dlya_soobsheniya_ob_oshibkah_primer_konvertatsii.xlsx
@@ -454,7 +454,7 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="2">
-        <v>43593</v>
+        <v>43593.71875</v>
       </c>
       <c r="B2" s="2">
         <v>43624</v>
@@ -477,7 +477,7 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="2">
-        <v>43563</v>
+        <v>43563.71875</v>
       </c>
       <c r="B3" s="2">
         <v>43593</v>

</xml_diff>

<commit_message>
prepared for v2.0. Minor changes
</commit_message>
<xml_diff>
--- a/Examples/primer_dlya_soobsheniya_ob_oshibkah_primer_konvertatsii.xlsx
+++ b/Examples/primer_dlya_soobsheniya_ob_oshibkah_primer_konvertatsii.xlsx
@@ -63,7 +63,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd.mm.yyyy"/>
+    <numFmt numFmtId="164" formatCode="dd.mm.yyyy HH:MM"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -454,10 +454,10 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="2">
-        <v>43593.71875</v>
+        <v>43682.71875</v>
       </c>
       <c r="B2" s="2">
-        <v>43624</v>
+        <v>43683</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -477,10 +477,10 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="2">
-        <v>43563.71875</v>
+        <v>43681.71875</v>
       </c>
       <c r="B3" s="2">
-        <v>43593</v>
+        <v>43682</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>

</xml_diff>